<commit_message>
Update DDU Kalender E2020 + F2021.xlsx
</commit_message>
<xml_diff>
--- a/DDU Kalender E2020 + F2021.xlsx
+++ b/DDU Kalender E2020 + F2021.xlsx
@@ -1374,7 +1374,7 @@
   <dimension ref="A1:AG32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3435,11 +3435,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="13">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="AB1:AD1"/>
     <mergeCell ref="AE1:AG1"/>
     <mergeCell ref="S30:U32"/>
     <mergeCell ref="J1:L1"/>
@@ -3448,6 +3443,11 @@
     <mergeCell ref="V1:X1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AB1:AD1"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157" right="0.39370078740157" top="0.39370078740157" bottom="0.39370078740157" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Update DDU Kalender E2020 + F2021.xlsx"
This reverts commit eda1e4e544b51577952668d172f1d4034b901e98.
</commit_message>
<xml_diff>
--- a/DDU Kalender E2020 + F2021.xlsx
+++ b/DDU Kalender E2020 + F2021.xlsx
@@ -1374,7 +1374,7 @@
   <dimension ref="A1:AG32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3435,6 +3435,11 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="13">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AB1:AD1"/>
     <mergeCell ref="AE1:AG1"/>
     <mergeCell ref="S30:U32"/>
     <mergeCell ref="J1:L1"/>
@@ -3443,11 +3448,6 @@
     <mergeCell ref="V1:X1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="AB1:AD1"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157" right="0.39370078740157" top="0.39370078740157" bottom="0.39370078740157" header="0.3" footer="0.3"/>

</xml_diff>